<commit_message>
refactor-monolith tested ok, about to pull into main
</commit_message>
<xml_diff>
--- a/scripts/dishesMenu.xlsx
+++ b/scripts/dishesMenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22755" windowHeight="8670" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22755" windowHeight="8670"/>
   </bookViews>
   <sheets>
     <sheet name="PriceList" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="139">
   <si>
     <t>Category</t>
   </si>
@@ -73,30 +73,12 @@
     <t>KIDS MENU</t>
   </si>
   <si>
-    <t>Cheeseburger, frites maison</t>
-  </si>
-  <si>
     <t>Mini Bouchée à la Reine maison</t>
   </si>
   <si>
-    <t>Nuggets de Poulet Maison</t>
-  </si>
-  <si>
     <t>12.50</t>
   </si>
   <si>
-    <t>Boule de glace Vanille</t>
-  </si>
-  <si>
-    <t>Boule de glace Chocolat</t>
-  </si>
-  <si>
-    <t>Boule de glace Citron</t>
-  </si>
-  <si>
-    <t>Boule de glace Fraise</t>
-  </si>
-  <si>
     <t>Sélection de glaces Fraise 1 boule</t>
   </si>
   <si>
@@ -220,9 +202,6 @@
     <t>Cheeseburger</t>
   </si>
   <si>
-    <t xml:space="preserve">small </t>
-  </si>
-  <si>
     <t>large</t>
   </si>
   <si>
@@ -440,6 +419,30 @@
   </si>
   <si>
     <t>Sauce BBQ</t>
+  </si>
+  <si>
+    <t>Kids Cheeseburger, frites maison</t>
+  </si>
+  <si>
+    <t>Kids Nuggets de Poulet Maison</t>
+  </si>
+  <si>
+    <t>Kids Boule de glace Vanille</t>
+  </si>
+  <si>
+    <t>Kids Boule de glace Chocolat</t>
+  </si>
+  <si>
+    <t>Kids Boule de glace Citron</t>
+  </si>
+  <si>
+    <t>Kids Boule de glace Fraise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">petite SOUPE du moment  </t>
+  </si>
+  <si>
+    <t>grande SOUPE du moment</t>
   </si>
 </sst>
 </file>
@@ -759,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,10 +789,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -797,10 +800,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,10 +811,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,10 +822,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -830,10 +833,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,10 +844,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -852,10 +855,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -863,10 +866,10 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -874,10 +877,10 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -885,10 +888,10 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -896,10 +899,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,10 +910,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -918,10 +921,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -929,10 +932,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
         <v>71</v>
-      </c>
-      <c r="C15" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -940,10 +943,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -951,10 +954,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,10 +965,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -973,10 +976,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -984,10 +987,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -995,10 +998,10 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1006,10 +1009,10 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1017,10 +1020,10 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1028,10 +1031,10 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,10 +1042,10 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1050,10 +1053,10 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1061,10 +1064,10 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1072,10 +1075,10 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1083,10 +1086,10 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1094,10 +1097,10 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1105,10 +1108,10 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1116,10 +1119,10 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1127,10 +1130,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1138,10 +1141,10 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1149,10 +1152,10 @@
         <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1160,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1171,10 +1174,10 @@
         <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1182,10 +1185,10 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1193,10 +1196,10 @@
         <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1204,10 +1207,10 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,10 +1218,10 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1226,10 +1229,10 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,10 +1240,10 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,10 +1251,10 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,10 +1262,10 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1270,10 +1273,10 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1281,10 +1284,10 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1292,10 +1295,10 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1303,10 +1306,10 @@
         <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1314,10 +1317,10 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1325,10 +1328,10 @@
         <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1336,10 +1339,10 @@
         <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1347,10 +1350,10 @@
         <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1369,10 +1372,10 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1380,10 +1383,10 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" t="s">
         <v>16</v>
-      </c>
-      <c r="C56" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1391,10 +1394,10 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1402,10 +1405,10 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>133</v>
       </c>
       <c r="C58" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1413,10 +1416,10 @@
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1424,10 +1427,10 @@
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="C60" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1435,10 +1438,10 @@
         <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>136</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1467,457 +1470,457 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" t="s">
         <v>97</v>
       </c>
-      <c r="C4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" t="s">
-        <v>104</v>
-      </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" t="s">
         <v>97</v>
       </c>
-      <c r="C5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" t="s">
-        <v>104</v>
-      </c>
       <c r="E5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
         <v>97</v>
       </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" t="s">
-        <v>104</v>
-      </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
         <v>97</v>
       </c>
-      <c r="C7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D7" t="s">
-        <v>104</v>
-      </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F9" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H16" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="H17" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G18" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E24" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1929,7 +1932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -1940,27 +1943,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add currency API route and update rate fetching logic
</commit_message>
<xml_diff>
--- a/scripts/dishesMenu.xlsx
+++ b/scripts/dishesMenu.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="142">
   <si>
     <t>Category</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Cheeseburger</t>
   </si>
   <si>
-    <t>large</t>
-  </si>
-  <si>
     <t>14.00</t>
   </si>
   <si>
@@ -443,6 +440,18 @@
   </si>
   <si>
     <t>grande SOUPE du moment</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>/images/camembertRoti.jpg</t>
+  </si>
+  <si>
+    <t>/images/cheeseburger.PNG</t>
+  </si>
+  <si>
+    <t>/images/doublecheeseburger.jpg</t>
   </si>
 </sst>
 </file>
@@ -760,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,9 +780,10 @@
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -783,272 +793,278 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
         <v>85</v>
       </c>
-      <c r="C5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
         <v>77</v>
       </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
         <v>75</v>
       </c>
-      <c r="C12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>73</v>
       </c>
-      <c r="C13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
         <v>70</v>
       </c>
-      <c r="C20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1058,8 +1074,11 @@
       <c r="C26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1069,8 +1088,11 @@
       <c r="C27" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1103,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1114,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1125,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1136,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1394,7 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
@@ -1394,7 +1416,7 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C57" t="s">
         <v>16</v>
@@ -1405,7 +1427,7 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C58" t="s">
         <v>18</v>
@@ -1416,7 +1438,7 @@
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C59" t="s">
         <v>18</v>
@@ -1427,7 +1449,7 @@
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
         <v>18</v>
@@ -1438,7 +1460,7 @@
         <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" t="s">
         <v>18</v>
@@ -1470,196 +1492,196 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
         <v>90</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>91</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>92</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>93</v>
-      </c>
-      <c r="F2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
         <v>90</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" t="s">
-        <v>93</v>
-      </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" t="s">
         <v>96</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" t="s">
         <v>97</v>
       </c>
-      <c r="E4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>98</v>
-      </c>
-      <c r="G4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" t="s">
         <v>96</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" t="s">
         <v>97</v>
       </c>
-      <c r="E5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>98</v>
-      </c>
-      <c r="G5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" t="s">
         <v>101</v>
-      </c>
-      <c r="D6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
         <v>101</v>
-      </c>
-      <c r="D7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>105</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>106</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>107</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>108</v>
-      </c>
-      <c r="G9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1667,19 +1689,19 @@
         <v>57</v>
       </c>
       <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
         <v>110</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>111</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>112</v>
       </c>
-      <c r="E11" t="s">
-        <v>113</v>
-      </c>
       <c r="F11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1687,19 +1709,19 @@
         <v>55</v>
       </c>
       <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
         <v>110</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>111</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>112</v>
       </c>
-      <c r="E12" t="s">
-        <v>113</v>
-      </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1707,16 +1729,16 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
         <v>118</v>
       </c>
-      <c r="C13" t="s">
-        <v>119</v>
-      </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1724,16 +1746,16 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1741,13 +1763,13 @@
         <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1755,25 +1777,25 @@
         <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" t="s">
         <v>114</v>
       </c>
-      <c r="D16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F16" t="s">
-        <v>93</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>115</v>
-      </c>
-      <c r="H16" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1781,25 +1803,25 @@
         <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" t="s">
         <v>114</v>
       </c>
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" t="s">
-        <v>113</v>
-      </c>
-      <c r="F17" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>115</v>
-      </c>
-      <c r="H17" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1807,22 +1829,22 @@
         <v>47</v>
       </c>
       <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
         <v>122</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>123</v>
       </c>
-      <c r="D18" t="s">
-        <v>124</v>
-      </c>
       <c r="E18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" t="s">
         <v>112</v>
       </c>
-      <c r="F18" t="s">
-        <v>113</v>
-      </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1830,10 +1852,10 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1841,10 +1863,10 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1852,13 +1874,13 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
+        <v>124</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="s">
         <v>125</v>
-      </c>
-      <c r="C21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1866,13 +1888,13 @@
         <v>35</v>
       </c>
       <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" t="s">
         <v>125</v>
-      </c>
-      <c r="C22" t="s">
-        <v>113</v>
-      </c>
-      <c r="D22" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1880,13 +1902,13 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1894,19 +1916,19 @@
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" t="s">
         <v>128</v>
-      </c>
-      <c r="F24" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1914,13 +1936,13 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>